<commit_message>
add PMMS rate, make national summary stats, update README
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aseII\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\covid-rent-study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B931567-05A7-463A-96E2-3036AB570AF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE4764D-B786-4989-87BA-62DE55B2FA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20724" yWindow="1008" windowWidth="18600" windowHeight="8964" xr2:uid="{D204D963-049D-4259-A844-F52802AEE347}"/>
+    <workbookView xWindow="2664" yWindow="1356" windowWidth="18600" windowHeight="8964" xr2:uid="{D204D963-049D-4259-A844-F52802AEE347}"/>
   </bookViews>
   <sheets>
     <sheet name="data-dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
   <si>
     <t>Variable</t>
   </si>
@@ -285,6 +285,24 @@
   </si>
   <si>
     <t>https://experience.arcgis.com/experience/dbbef7041b104215a7442606f0897836/</t>
+  </si>
+  <si>
+    <t>Average mortgage rate</t>
+  </si>
+  <si>
+    <t>Freddie Mac PMMS</t>
+  </si>
+  <si>
+    <t>pmms_rate</t>
+  </si>
+  <si>
+    <t>Primary Mortgage Market Survey rate</t>
+  </si>
+  <si>
+    <t>Freddis Mac</t>
+  </si>
+  <si>
+    <t>http://www.freddiemac.com/pmms/docs/PMMS_history.csv</t>
   </si>
 </sst>
 </file>
@@ -359,6 +377,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED77F026-E462-44D0-A686-95A86EF0A150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7208520" y="0"/>
+          <a:ext cx="6606540" cy="2567940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,16 +742,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F63AA7-06B9-4D37-BD71-FB25C581CC0A}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" customWidth="1"/>
@@ -1161,6 +1246,26 @@
       </c>
       <c r="G23" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43101</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44228</v>
+      </c>
+      <c r="E24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E24C2E-2728-4341-9074-01105AA4E0BA}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,21 +1492,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>83</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44214</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44307</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>53</v>
@@ -1415,21 +1520,21 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>53</v>
@@ -1443,7 +1548,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>53</v>
@@ -1452,25 +1557,40 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add all final changes
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\covid-rent-study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE4764D-B786-4989-87BA-62DE55B2FA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A8475-6278-47C2-9BD1-8C5B26FCEB16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2664" yWindow="1356" windowWidth="18600" windowHeight="8964" xr2:uid="{D204D963-049D-4259-A844-F52802AEE347}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D204D963-049D-4259-A844-F52802AEE347}"/>
   </bookViews>
   <sheets>
     <sheet name="data-dictionary" sheetId="1" r:id="rId1"/>
     <sheet name="rural-classification-codes" sheetId="2" r:id="rId2"/>
-    <sheet name="data-dictionary_paper" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>Variable</t>
   </si>
@@ -230,24 +229,9 @@
     <t>Nonmetro - Urban population of 20,000 or more, not adjacent to a metro area</t>
   </si>
   <si>
-    <t>Zillow Home Value Index</t>
-  </si>
-  <si>
-    <t>COVID State executive orders</t>
-  </si>
-  <si>
-    <t>Indiana University/Univeristy of Miami</t>
-  </si>
-  <si>
-    <t>State gubernatorial party</t>
-  </si>
-  <si>
     <t>Zillow</t>
   </si>
   <si>
-    <t>Apartment List</t>
-  </si>
-  <si>
     <t>zhvi</t>
   </si>
   <si>
@@ -287,22 +271,16 @@
     <t>https://experience.arcgis.com/experience/dbbef7041b104215a7442606f0897836/</t>
   </si>
   <si>
-    <t>Average mortgage rate</t>
-  </si>
-  <si>
-    <t>Freddie Mac PMMS</t>
-  </si>
-  <si>
     <t>pmms_rate</t>
   </si>
   <si>
     <t>Primary Mortgage Market Survey rate</t>
   </si>
   <si>
-    <t>Freddis Mac</t>
-  </si>
-  <si>
     <t>http://www.freddiemac.com/pmms/docs/PMMS_history.csv</t>
+  </si>
+  <si>
+    <t>Freddie Mac</t>
   </si>
 </sst>
 </file>
@@ -334,7 +312,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -342,26 +320,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,72 +344,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED77F026-E462-44D0-A686-95A86EF0A150}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7208520" y="0"/>
-          <a:ext cx="6606540" cy="2567940"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,7 +646,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,10 +744,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1">
         <v>43101</v>
@@ -855,10 +756,10 @@
         <v>44228</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -866,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1">
         <v>43101</v>
@@ -875,10 +776,10 @@
         <v>44228</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -886,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1">
         <v>43101</v>
@@ -895,10 +796,10 @@
         <v>44228</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1190,10 +1091,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>53</v>
@@ -1202,58 +1103,58 @@
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
         <v>76</v>
       </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
-      </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" t="s">
         <v>77</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1">
         <v>43101</v>
@@ -1262,10 +1163,10 @@
         <v>44228</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1374,223 +1275,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E24C2E-2728-4341-9074-01105AA4E0BA}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43101</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44276</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44214</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44276</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43831</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44228</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43891</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44287</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43891</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44287</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43770</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44228</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44214</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44307</v>
-      </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>